<commit_message>
Cleanup meshes with stricter rules
</commit_message>
<xml_diff>
--- a/res/final/reports/camerafocus.xlsx
+++ b/res/final/reports/camerafocus.xlsx
@@ -294,13 +294,13 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
-      <rgbColor rgb="FF579D1C"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -326,7 +326,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$H$1</c:f>
+              <c:f>Sheet!$H$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -357,21 +357,6 @@
             <c:showPercent val="0"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet!$A$2:$A$33</c:f>
@@ -379,100 +364,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>-38</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-36</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-34</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-32</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-30</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-28</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-26</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-24</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-18</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-16</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-14</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-12</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-8</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-6</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6</c:v>
+                  <c:v>-6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8</c:v>
+                  <c:v>-8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12</c:v>
+                  <c:v>-12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14</c:v>
+                  <c:v>-14</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>16</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>18</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>22</c:v>
+                  <c:v>-22</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>24</c:v>
+                  <c:v>-24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,100 +469,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.100427957085097</c:v>
+                  <c:v>0.567990517665866</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.101770844582635</c:v>
+                  <c:v>0.536015691093296</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0977193600927419</c:v>
+                  <c:v>0.489887470353219</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.100865591906702</c:v>
+                  <c:v>0.437145137935217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0919678689143898</c:v>
+                  <c:v>0.39346178478576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0905844862340297</c:v>
+                  <c:v>0.323980320575023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0918371925035394</c:v>
+                  <c:v>0.304414579861668</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0892592747429614</c:v>
+                  <c:v>0.291332781582688</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0850179864233004</c:v>
+                  <c:v>0.250996469558965</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0858814543544554</c:v>
+                  <c:v>0.200367567200889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0797884048491999</c:v>
+                  <c:v>0.187201186207308</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0782024240324357</c:v>
+                  <c:v>0.136117826116269</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0784403746811164</c:v>
+                  <c:v>0.135567581247601</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0765472475726058</c:v>
+                  <c:v>0.114038494249715</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0753809174724721</c:v>
+                  <c:v>0.0569288345591843</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0682451174201603</c:v>
+                  <c:v>0.0213390468342521</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0724077778776273</c:v>
+                  <c:v>0.0363746255074098</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.064075876119721</c:v>
+                  <c:v>0.00790319085873749</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0653943866957135</c:v>
+                  <c:v>0.0222766353972845</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0617130556593841</c:v>
+                  <c:v>0.0364057705082286</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0610810016581736</c:v>
+                  <c:v>0.0120185286221493</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0598976132100856</c:v>
+                  <c:v>0.0403357163471919</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.060135335288394</c:v>
+                  <c:v>0.0134651973767044</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.0600920541707524</c:v>
+                  <c:v>0.0394709326988054</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0740653190110797</c:v>
+                  <c:v>0.0631007602347951</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0794699507971298</c:v>
+                  <c:v>0.0825170352992368</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0963682803659466</c:v>
+                  <c:v>0.100646448689098</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.10632847937556</c:v>
+                  <c:v>0.131351801333952</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.122113688711111</c:v>
+                  <c:v>0.161078707428293</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.126842303308703</c:v>
+                  <c:v>0.195427284636176</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.123265420264086</c:v>
+                  <c:v>0.22826398989182</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.113729961989319</c:v>
+                  <c:v>0.271925281593608</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,22 +574,22 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet!$L$1</c:f>
+              <c:f>Sheet!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mean Curvature avg</c:v>
+                  <c:v>Mean Curvature std</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ffd320"/>
+              <a:srgbClr val="ff420e"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="ffd320"/>
+                <a:srgbClr val="ff420e"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -627,363 +612,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>-38</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-36</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-34</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-32</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-30</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-28</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-26</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-24</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-22</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-18</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-16</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-14</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-12</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-10</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-8</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-6</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6</c:v>
+                  <c:v>-6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8</c:v>
+                  <c:v>-8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>10</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12</c:v>
+                  <c:v>-12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14</c:v>
+                  <c:v>-14</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>16</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>18</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>22</c:v>
+                  <c:v>-22</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet!$L$2:$L$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
-                <c:pt idx="0">
-                  <c:v>7.54208056868815E-006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.38184097297977E-006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.000151202106893832</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.00024972458325059</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.56571952689001E-005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.00016890369932299</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.000182525117061953</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.62871918204059E-005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.55114954924846E-006</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.000190988724908012</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.86126290972799E-005</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.63674111363453E-005</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.000239260803318635</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.000193484162217485</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.47732835099154E-005</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.000154915928499174</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.000174722292986179</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.000240350215686193</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.75507791619359E-005</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.17600873276681E-005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.000228162011388314</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.000274726574586657</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.000206953546899324</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.000642630334614898</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.00101296974478237</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.000612032941005047</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.00135313227447882</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.00167257309475441</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.00142649477463418</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.00132010840040197</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.00203577068523904</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.00296275156398858</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet!$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mean Curvature std</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="579d1c"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet!$A$2:$A$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
-                <c:pt idx="0">
-                  <c:v>-38</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-36</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-34</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-28</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-26</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>-24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-22</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-16</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-12</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1095,11 +817,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="60469675"/>
-        <c:axId val="13224325"/>
+        <c:axId val="70095177"/>
+        <c:axId val="21054706"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60469675"/>
+        <c:axId val="70095177"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1134,12 +856,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13224325"/>
+        <c:crossAx val="21054706"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13224325"/>
+        <c:axId val="21054706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1183,8 +905,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60469675"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="70095177"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1224,16 +946,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>255600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1640160</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>196560</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1241,8 +963,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1308600" y="6295680"/>
-        <a:ext cx="8559000" cy="6849000"/>
+        <a:off x="4027320" y="6525000"/>
+        <a:ext cx="7484760" cy="6076800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1262,20 +984,13 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.2955465587045"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.165991902834"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.29959514170041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.3481781376518"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.3967611336032"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8461538461538"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,7 +1036,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>-38</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>13</v>
@@ -1330,42 +1045,42 @@
         <v>2520</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>253.078451854445</v>
+        <v>1431.33610451798</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>0.100427957085097</v>
+        <v>0.567990517665866</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0.159543644354881</v>
+        <v>0.159488103591829</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>4.21842112367803</v>
+        <v>150.74042709441</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>7.54208056868815E-006</v>
+        <v>7.45550327337433E-006</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>0.00739221935119033</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>-319.755672037543</v>
+        <v>946.411402262428</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>-36</v>
+        <v>36</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>14</v>
@@ -1374,42 +1089,42 @@
         <v>2578</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>262.365237334034</v>
+        <v>1381.84845163852</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0.101770844582635</v>
+        <v>0.536015691093296</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0.162407978431478</v>
+        <v>0.162362245969606</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>3.67659495968958</v>
+        <v>129.380270381181</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>9.38184097297977E-006</v>
+        <v>9.29526367766595E-006</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>0.00795929551689418</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>-300.073310835907</v>
+        <v>959.343698829915</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>-34</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
@@ -1418,42 +1133,42 @@
         <v>2653</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>259.249462326044</v>
+        <v>1299.67145884709</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>0.0977193600927419</v>
+        <v>0.489887470353219</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>0.163457178010336</v>
+        <v>0.163415899162615</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>3.30874779685331</v>
+        <v>127.329221758436</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>0.000151202106893832</v>
+        <v>0.000151115529598518</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>0.00813613683594722</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>-280.066620793052</v>
+        <v>972.69715589618</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>-32</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>16</v>
@@ -1462,42 +1177,42 @@
         <v>2721</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>274.455275578137</v>
+        <v>1189.47192032173</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>0.100865591906702</v>
+        <v>0.437145137935217</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>0.186091554696233</v>
+        <v>0.186057261755549</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>5.82526914135113</v>
+        <v>238.686661492128</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>0.00024972458325059</v>
+        <v>0.000249638005955276</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>0.00890169366412051</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>-260.572537140705</v>
+        <v>985.950534891121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>17</v>
@@ -1506,42 +1221,42 @@
         <v>2777</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>255.39477197526</v>
+        <v>1092.64337635006</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>0.0919678689143898</v>
+        <v>0.39346178478576</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>0.164513863732603</v>
+        <v>0.164466857106724</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>5.36845209060435</v>
+        <v>103.999001198135</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>2.56571952689001E-005</v>
+        <v>2.57437725642139E-005</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>0.00741525461017986</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>-240.841404369409</v>
+        <v>999.587594456374</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>-28</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
@@ -1550,42 +1265,42 @@
         <v>2854</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>258.528123711921</v>
+        <v>924.639834921115</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.0905844862340297</v>
+        <v>0.323980320575023</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>0.130285240029185</v>
+        <v>0.130208239251434</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>1.99668295446199</v>
+        <v>84.9789939877129</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>0.00016890369932299</v>
+        <v>0.000168817122027676</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>0.0072830316215163</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>-220.528808571376</v>
+        <v>1013.81121239239</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>-26</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>19</v>
@@ -1594,42 +1309,42 @@
         <v>2923</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>268.440113687845</v>
+        <v>889.803816935656</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0.0918371925035394</v>
+        <v>0.304414579861668</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>0.154298821398029</v>
+        <v>0.154238418772696</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>5.58557520204995</v>
+        <v>64.0177813628052</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>0.000182525117061953</v>
+        <v>0.000182438539766639</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>0.00931991975363487</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>-200.658282563213</v>
+        <v>1027.95045888171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>-24</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>20</v>
@@ -1638,42 +1353,42 @@
         <v>3022</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>269.741528273229</v>
+        <v>880.407665942882</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>0.0892592747429614</v>
+        <v>0.291332781582688</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>0.138852609094524</v>
+        <v>0.138797554953761</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>2.52228738313354</v>
+        <v>65.4577378647282</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>8.62871918204059E-005</v>
+        <v>8.63737691157197E-005</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>0.00765499854105232</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>-180.401822731715</v>
+        <v>1042.54510185561</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>-22</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>21</v>
@@ -1682,42 +1397,42 @@
         <v>3064</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>260.495110400992</v>
+        <v>769.05318272867</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>0.0850179864233004</v>
+        <v>0.250996469558965</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>0.124064727206617</v>
+        <v>0.123992384441857</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>2.35010815214106</v>
+        <v>44.5434335326754</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>6.55114954924846E-006</v>
+        <v>6.63772684456228E-006</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>0.00833116816426023</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>-160.436878147366</v>
+        <v>1057.11836696095</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>-20</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>22</v>
@@ -1726,42 +1441,42 @@
         <v>3179</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>273.017143392814</v>
+        <v>636.968496131626</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>0.0858814543544554</v>
+        <v>0.200367567200889</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>0.127721200516969</v>
+        <v>0.127648373677649</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>2.13177181023279</v>
+        <v>29.8520953597422</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>0.000190988724908012</v>
+        <v>0.000190902147612698</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>0.00721593931397929</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>-140.688663048421</v>
+        <v>1071.7455597932</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>-18</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>23</v>
@@ -1770,42 +1485,42 @@
         <v>3247</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>259.072950545352</v>
+        <v>607.842251615129</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.0797884048491999</v>
+        <v>0.187201186207308</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>0.119407381354757</v>
+        <v>0.119335957108011</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>1.9814837454837</v>
+        <v>11.2068108346562</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>7.86126290972799E-005</v>
+        <v>7.85260518019661E-005</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>0.00728833568538214</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>-120.395811045763</v>
+        <v>1087.04691337302</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>-16</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>24</v>
@@ -1814,42 +1529,42 @@
         <v>3322</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>259.788452635751</v>
+        <v>452.183418358245</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.0782024240324357</v>
+        <v>0.136117826116269</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>0.128765338011279</v>
+        <v>0.128704292217558</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>4.37480558640681</v>
+        <v>35.3928846776075</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>5.63674111363453E-005</v>
+        <v>5.62808338410315E-005</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>0.00665224202911688</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>-100.78222525859</v>
+        <v>1101.66335050762</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>-14</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>25</v>
@@ -1858,42 +1573,42 @@
         <v>3429</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>268.972044781548</v>
+        <v>464.861236098025</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>0.0784403746811164</v>
+        <v>0.135567581247601</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>0.13475075445332</v>
+        <v>0.134694588601377</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>4.91535114716018</v>
+        <v>13.9414872869399</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>0.000239260803318635</v>
+        <v>0.000239174226023322</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>0.00793462131247061</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>-80.8494912246168</v>
+        <v>1116.83516728008</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>-12</v>
+        <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>26</v>
@@ -1902,42 +1617,42 @@
         <v>3523</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>269.67595319829</v>
+        <v>401.757615241747</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>0.0765472475726058</v>
+        <v>0.114038494249715</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>0.136771605197143</v>
+        <v>0.136716981383275</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>5.81158836639155</v>
+        <v>19.0915179633153</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>0.000193484162217485</v>
+        <v>0.000193397584922171</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>0.00819766781071763</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>-60.9187555652473</v>
+        <v>1132.20165440342</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>27</v>
@@ -1946,42 +1661,42 @@
         <v>3699</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>278.834013730674</v>
+        <v>210.579759034423</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>0.0753809174724721</v>
+        <v>0.0569288345591843</v>
       </c>
       <c r="I16" s="0" t="n">
-        <v>0.178703656108278</v>
+        <v>0.178667986601757</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>6.6220910956314</v>
+        <v>47.7167289184562</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>7.47732835099154E-005</v>
+        <v>7.46867062146016E-005</v>
       </c>
       <c r="M16" s="0" t="n">
         <v>0.0060391774310833</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>-21.1271489402931</v>
+        <v>1163.26384542357</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>28</v>
@@ -1990,42 +1705,42 @@
         <v>3805</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>259.67267178371</v>
+        <v>81.1950732043293</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>0.0682451174201603</v>
+        <v>0.0213390468342521</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>0.114713836096253</v>
+        <v>0.114653472827332</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>3.43467576561986</v>
+        <v>31.1195956085515</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>0.000154915928499174</v>
+        <v>0.00015482935120386</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>0.00603181038778358</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>-1.14661750910367</v>
+        <v>1179.06966870278</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>29</v>
@@ -2034,42 +1749,42 @@
         <v>3925</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>284.200528169687</v>
+        <v>142.770405116583</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>0.0724077778776273</v>
+        <v>0.0363746255074098</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>0.167742503398671</v>
+        <v>0.167713608835667</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>5.64985364235227</v>
+        <v>39.4396670830892</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>0.000174722292986179</v>
+        <v>0.000174635715690865</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>0.00685470080679428</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>18.8266172468831</v>
+        <v>1195.00508084334</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>30</v>
@@ -2078,42 +1793,42 @@
         <v>4020</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>257.585022001279</v>
+        <v>31.7708272521247</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0.064075876119721</v>
+        <v>0.00790319085873749</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>0.131457208593461</v>
+        <v>0.131412467033307</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>6.4084701853166</v>
+        <v>18.9364607087923</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>0.000240350215686193</v>
+        <v>0.000240263638390879</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>0.00782005706233514</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>38.873247043732</v>
+        <v>1211.09008846979</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>31</v>
@@ -2122,37 +1837,37 @@
         <v>4123</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>269.621056346427</v>
+        <v>91.8465677430039</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>0.0653943866957135</v>
+        <v>0.0222766353972845</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>0.143409390457214</v>
+        <v>0.143379682116858</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>4.08284873750613</v>
+        <v>61.6894350778072</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>6.75507791619359E-005</v>
+        <v>6.74642018666221E-005</v>
       </c>
       <c r="M20" s="0" t="n">
         <v>0.00644371248659801</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>58.2277541633618</v>
+        <v>1226.78422496866</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,42 +1881,42 @@
         <v>4237</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>261.478216828811</v>
+        <v>154.251249643365</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>0.0617130556593841</v>
+        <v>0.0364057705082286</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>0.134467125463033</v>
+        <v>0.134434645631726</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>5.47255809416347</v>
+        <v>99.8314993644344</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>3.17600873276681E-005</v>
+        <v>3.16735100323543E-005</v>
       </c>
       <c r="M21" s="0" t="n">
         <v>0.00665464384273301</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>76.4633270328651</v>
+        <v>1242.19643796241</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>33</v>
@@ -2210,42 +1925,42 @@
         <v>4319</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>263.808846161652</v>
+        <v>51.9080251190626</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>0.0610810016581736</v>
+        <v>0.0120185286221493</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>0.159837954075227</v>
+        <v>0.15981995818098</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>5.69229022404026</v>
+        <v>50.8492544795057</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>0.000228162011388314</v>
+        <v>0.000228075434093001</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>0.0067833131669933</v>
       </c>
       <c r="N22" s="0" t="n">
-        <v>97.3753919718955</v>
+        <v>1259.29635778328</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>34</v>
@@ -2254,42 +1969,42 @@
         <v>4405</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>263.848986190427</v>
+        <v>177.67883050938</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>0.0598976132100856</v>
+        <v>0.0403357163471919</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>0.143711033884548</v>
+        <v>0.143696133585487</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>4.71130761092121</v>
+        <v>138.913328155094</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>0.000274726574586657</v>
+        <v>0.000274639997291343</v>
       </c>
       <c r="M23" s="0" t="n">
         <v>0.008471425925113</v>
       </c>
       <c r="N23" s="0" t="n">
-        <v>117.294824500128</v>
+        <v>1275.72267589399</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>35</v>
@@ -2298,42 +2013,42 @@
         <v>4458</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>268.083324715661</v>
+        <v>60.0278499053483</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>0.060135335288394</v>
+        <v>0.0134651973767044</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>0.135948283963054</v>
+        <v>0.135938148201365</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>3.95222775351593</v>
+        <v>57.4043003601668</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>0.000206953546899324</v>
+        <v>0.00020686696960401</v>
       </c>
       <c r="M24" s="0" t="n">
         <v>0.00969457278954451</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>137.265276382121</v>
+        <v>1291.72680062892</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>36</v>
@@ -2342,42 +2057,42 @@
         <v>4402</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>264.525222459652</v>
+        <v>173.751045740141</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>0.0600920541707524</v>
+        <v>0.0394709326988054</v>
       </c>
       <c r="I25" s="0" t="n">
-        <v>0.117678985500708</v>
+        <v>0.117655009012347</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>4.8519862768436</v>
+        <v>171.80463939363</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>0.000642630334614898</v>
+        <v>0.000642543757319584</v>
       </c>
       <c r="M25" s="0" t="n">
         <v>0.0110093220672061</v>
       </c>
       <c r="N25" s="0" t="n">
-        <v>157.539313525926</v>
+        <v>1308.67325095405</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>37</v>
@@ -2386,42 +2101,42 @@
         <v>4283</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>317.221761324454</v>
+        <v>270.260556085627</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>0.0740653190110797</v>
+        <v>0.0631007602347951</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>0.152699434402558</v>
+        <v>0.152677544344417</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>4.04872811974185</v>
+        <v>167.84171666336</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>0.00101296974478237</v>
+        <v>0.00101288316748706</v>
       </c>
       <c r="M26" s="0" t="n">
         <v>0.0135328787521979</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>177.597617249445</v>
+        <v>1325.55640854645</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>38</v>
@@ -2430,42 +2145,42 @@
         <v>4114</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>326.939377579392</v>
+        <v>339.47508322106</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>0.0794699507971298</v>
+        <v>0.0825170352992368</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>0.170483964609326</v>
+        <v>0.170477847335014</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>4.98407153057188</v>
+        <v>187.001721822015</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>0.000612032941005047</v>
+        <v>0.000611946363709733</v>
       </c>
       <c r="M27" s="0" t="n">
         <v>0.0158392454814995</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>198.607765021444</v>
+        <v>1343.27557724028</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>14</v>
+        <v>-14</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>39</v>
@@ -2474,42 +2189,42 @@
         <v>3970</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>382.582073052808</v>
+        <v>399.56640129572</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>0.0963682803659466</v>
+        <v>0.100646448689098</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>0.17910299360773</v>
+        <v>0.179089639393158</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>6.05658534354814</v>
+        <v>207.984576020054</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>0.00135313227447882</v>
+        <v>0.0013530456971835</v>
       </c>
       <c r="M28" s="0" t="n">
         <v>0.0207045109800706</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>218.366253054276</v>
+        <v>1360.07339541176</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>40</v>
@@ -2518,42 +2233,42 @@
         <v>3740</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>397.668512864593</v>
+        <v>491.255736988982</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>0.10632847937556</v>
+        <v>0.131351801333952</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>0.156121434896035</v>
+        <v>0.156092068764835</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>2.95447701516991</v>
+        <v>208.430654787506</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>0.00167257309475441</v>
+        <v>0.0016724865174591</v>
       </c>
       <c r="M29" s="0" t="n">
         <v>0.0225809038845651</v>
       </c>
       <c r="N29" s="0" t="n">
-        <v>238.487737608557</v>
+        <v>1377.21183458546</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>18</v>
+        <v>-18</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>41</v>
@@ -2562,42 +2277,42 @@
         <v>3593</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>438.754483539022</v>
+        <v>578.755795789856</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>0.122113688711111</v>
+        <v>0.161078707428293</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>0.211725644572428</v>
+        <v>0.211713072792598</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>4.7692026908036</v>
+        <v>222.182845297246</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>0.00142649477463418</v>
+        <v>0.00142640819733886</v>
       </c>
       <c r="M30" s="0" t="n">
         <v>0.0268370319042657</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>258.677676366643</v>
+        <v>1394.54877631623</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>42</v>
@@ -2606,42 +2321,42 @@
         <v>3375</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>428.092773666873</v>
+        <v>659.567085647096</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>0.126842303308703</v>
+        <v>0.195427284636176</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>0.202255647187166</v>
+        <v>0.202240882438945</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>4.00354572106798</v>
+        <v>232.586547166352</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>0.00132010840040197</v>
+        <v>0.00132002182310666</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>0.0301923293591107</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>279.02298386419</v>
+        <v>1412.06229125813</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>22</v>
+        <v>-22</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>43</v>
@@ -2650,42 +2365,42 @@
         <v>3185</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>392.600363541113</v>
+        <v>727.020807805447</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>0.123265420264086</v>
+        <v>0.22826398989182</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>0.191894164727029</v>
+        <v>0.191880545179089</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>3.43888786256674</v>
+        <v>239.064937152032</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>0.00203577068523904</v>
+        <v>0.00203568410794373</v>
       </c>
       <c r="M32" s="0" t="n">
         <v>0.0319151793900287</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>298.404757437486</v>
+        <v>1428.79032945238</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>24</v>
+        <v>-24</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>44</v>
@@ -2694,37 +2409,37 @@
         <v>3090</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>80.065605</v>
+        <v>80.06505</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>351.425582546997</v>
+        <v>840.249120124248</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>0.113729961989319</v>
+        <v>0.271925281593608</v>
       </c>
       <c r="I33" s="0" t="n">
-        <v>0.174619157346615</v>
+        <v>0.174603013108534</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>4.91056351197713</v>
+        <v>257.212497238813</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>0.0124897576181433</v>
+        <v>0.0124898441954386</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>0.00296275156398858</v>
+        <v>0.00296266498669327</v>
       </c>
       <c r="M33" s="0" t="n">
         <v>0.0499938019525503</v>
       </c>
       <c r="N33" s="0" t="n">
-        <v>318.213507313364</v>
+        <v>1445.97467067518</v>
       </c>
     </row>
   </sheetData>
@@ -2814,7 +2529,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>